<commit_message>
COMPLETE CONNECT TO GOOGLE SHEETS
</commit_message>
<xml_diff>
--- a/resources/privates/data.xlsx
+++ b/resources/privates/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AD\Desktop\BOT_LINKEDIN\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AD\Desktop\BOT_LINKEDIN\resources\privates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E663C9-D6F7-4568-986D-F0D0E3A40C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2A893-E0B2-4A65-8691-EB0D626898EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>LINKEDIN_LINK</t>
   </si>
@@ -41,29 +41,6 @@
   </si>
   <si>
     <t>ATTACHMENT</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/quan-tran-1574a4233/</t>
-  </si>
-  <si>
-    <t>Connected</t>
-  </si>
-  <si>
-    <t>Message sent</t>
-  </si>
-  <si>
-    <t>Quan Tran</t>
-  </si>
-  <si>
-    <t>Funding services with USD $900+ trillion option leadership
-Dear {{name}},
-Let's exchange your funding cost for equity by adding the huge benefit of tokenization + cross-border payment climate change Compound Options to your scaling business.
-Funding cost is 15+% for the funding amount less than USD $10 billion, at least USD $1 million.
-The SIGNIFICANTLY cheaper way is donating to TAHK Foundation for enjoying USD $900+ trillion option leadership, then I will help you with your target:
-- Donating $150 thousand USD per year service.
-- Email to donate@tahkfoundation.org for your donation.
-As an Universal Interacting &amp; Media Solutions nonprofit, TAHK Foundation will help you interact with best options for your requirements.
-Best regards,</t>
   </si>
 </sst>
 </file>
@@ -411,18 +388,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.77734375" customWidth="1"/>
+    <col min="2" max="7" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -448,26 +423,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>